<commit_message>
Fix syntax on MCA_Belaege_Szenario1 and generated code for MCA Belaege Szenario 1 bis 3
</commit_message>
<xml_diff>
--- a/00_data_raw/Belaege_Gewichtung_Szenario1.xlsx
+++ b/00_data_raw/Belaege_Gewichtung_Szenario1.xlsx
@@ -5,22 +5,23 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zhaw-my.sharepoint.com/personal/pfeifsar_students_zhaw_ch/Documents/6. Semester MSc UnR/Thesis/R_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zhaw-my.sharepoint.com/personal/pfeifsar_students_zhaw_ch/Documents/6. Semester MSc UnR/Thesis/R_Project/00_data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{72486D78-DEF3-48B5-ABEC-3983F2E8BA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03428A39-C63E-49F1-8C0E-8898EC50EE13}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{72486D78-DEF3-48B5-ABEC-3983F2E8BA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47CB1B56-9D4B-40D7-9328-3D5FBFEA96D5}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-34710" yWindow="2340" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19305" yWindow="-1350" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Gewichtung" sheetId="1" r:id="rId1"/>
+    <sheet name="Begründung" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>group_id</t>
   </si>
@@ -137,6 +138,11 @@
   </si>
   <si>
     <t>modulareErneuerbarkeit</t>
+  </si>
+  <si>
+    <t>Szenario 1: "Ausgewogene Nachhaltigkeit" (Baseline)
+Szenario 1, "Ausgewogene Nachhaltigkeit", dient als Baseline-Szenario. Die Gewichtung (Umweltbelastung: 30%; Langlebigkeit &amp; Wirtschaftlichkeit: 25%; Multifunktionale Nutzungsqualität: 25%; Kreislauffähigkeit: 20%) repräsentiert einen holistischen Ansatz, bei dem alle vier zentralen Bewertungsbereiche annähernd gleich stark priorisiert werden.
+Diese Verteilung legitimiert sich direkt aus Forschungsziel 1, welches eine umfassende Analyse von Umweltverträglichkeit, Lebensdauer und Kreislauffähigkeit fordert, sowie Forschungsziel 2, das die Anwendung eines breiten Bewertungsrasters impliziert. Das Szenario bildet die Referenz, an der die Sensitivität der Prioritätenverschiebung in den Folgeszenarien gemessen wird.</t>
   </si>
 </sst>
 </file>
@@ -195,10 +201,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -827,4 +836,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19AB53B4-2FBE-46B8-B527-F1B1CE8FDF72}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="53.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add szenario 0, fix render figures
</commit_message>
<xml_diff>
--- a/00_data_raw/Belaege_Gewichtung_Szenario1.xlsx
+++ b/00_data_raw/Belaege_Gewichtung_Szenario1.xlsx
@@ -8,20 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zhaw-my.sharepoint.com/personal/pfeifsar_students_zhaw_ch/Documents/6. Semester MSc UnR/Thesis/R_Project/00_data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{72486D78-DEF3-48B5-ABEC-3983F2E8BA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47CB1B56-9D4B-40D7-9328-3D5FBFEA96D5}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{72486D78-DEF3-48B5-ABEC-3983F2E8BA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93392BD8-8E64-4C26-BB3D-14B844453444}"/>
   <bookViews>
-    <workbookView xWindow="-19305" yWindow="-1350" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19305" yWindow="-1350" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gewichtung" sheetId="1" r:id="rId1"/>
     <sheet name="Begründung" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>group_id</t>
   </si>
@@ -39,9 +52,6 @@
   </si>
   <si>
     <t>within_group_weight</t>
-  </si>
-  <si>
-    <t>total_weight</t>
   </si>
   <si>
     <t>umweltbelastung</t>
@@ -519,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -553,284 +563,249 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2">
-        <v>0.6</v>
-      </c>
-      <c r="G2">
-        <v>0.18</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3">
-        <v>0.4</v>
-      </c>
-      <c r="G3">
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4">
-        <v>0.4</v>
-      </c>
-      <c r="G4">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5">
-        <v>0.3</v>
-      </c>
-      <c r="G5">
-        <v>7.4999999999999997E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6">
-        <v>0.3</v>
-      </c>
-      <c r="G6">
-        <v>7.4999999999999997E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7">
-        <v>0.3</v>
-      </c>
-      <c r="G7">
-        <v>7.4999999999999997E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8">
-        <v>0.3</v>
-      </c>
-      <c r="G8">
-        <v>7.4999999999999997E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9">
-        <v>0.2</v>
-      </c>
-      <c r="G9">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10">
-        <v>0.2</v>
-      </c>
-      <c r="G10">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11">
-        <v>0.4</v>
-      </c>
-      <c r="G11">
-        <v>0.08</v>
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12">
-        <v>0.3</v>
-      </c>
-      <c r="G12">
-        <v>0.06</v>
+        <f t="shared" ref="F12:F13" si="0">1/3</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13">
-        <v>0.3</v>
-      </c>
-      <c r="G13">
-        <v>0.06</v>
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
   </sheetData>
@@ -842,7 +817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19AB53B4-2FBE-46B8-B527-F1B1CE8FDF72}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -853,7 +828,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>